<commit_message>
kgcontroller and commit html
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,62 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>foresatt_pnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -648,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,6 +721,19 @@
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>barn_pnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -679,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +818,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2024-11-06</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>